<commit_message>
Changes format of occupancy KPIs with Wi-Fi device count data: Typical arrival times and departure times are now outputted in the format hh:mm; previously just number of hours past midnight.
</commit_message>
<xml_diff>
--- a/toolkit/outputs/6-occupancy/arrive_depart_maxOcc.xlsx
+++ b/toolkit/outputs/6-occupancy/arrive_depart_maxOcc.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="15">
   <si>
     <t>tArr_wkdy</t>
   </si>
@@ -32,6 +32,33 @@
   </si>
   <si>
     <t>sOcc_wknd</t>
+  </si>
+  <si>
+    <t>08:00</t>
+  </si>
+  <si>
+    <t>07:00</t>
+  </si>
+  <si>
+    <t>19:00</t>
+  </si>
+  <si>
+    <t>21:00</t>
+  </si>
+  <si>
+    <t>20:00</t>
+  </si>
+  <si>
+    <t>18:00</t>
+  </si>
+  <si>
+    <t>09:00</t>
+  </si>
+  <si>
+    <t>10:00</t>
+  </si>
+  <si>
+    <t>12:00</t>
   </si>
 </sst>
 </file>
@@ -419,11 +446,11 @@
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
         <v>8</v>
-      </c>
-      <c r="C2">
-        <v>19</v>
       </c>
       <c r="D2">
         <v>24</v>
@@ -436,20 +463,20 @@
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>7</v>
-      </c>
-      <c r="C3">
-        <v>19</v>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
       </c>
       <c r="D3">
         <v>56</v>
       </c>
-      <c r="E3">
-        <v>7</v>
-      </c>
-      <c r="F3">
-        <v>19</v>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>8</v>
       </c>
       <c r="G3">
         <v>9</v>
@@ -459,20 +486,20 @@
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>7</v>
-      </c>
-      <c r="C4">
-        <v>21</v>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
       </c>
       <c r="D4">
         <v>32</v>
       </c>
-      <c r="E4">
-        <v>9</v>
-      </c>
-      <c r="F4">
-        <v>20</v>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
       </c>
       <c r="G4">
         <v>11</v>
@@ -482,20 +509,20 @@
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5">
-        <v>7</v>
-      </c>
-      <c r="C5">
-        <v>19</v>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
       </c>
       <c r="D5">
         <v>89</v>
       </c>
-      <c r="E5">
-        <v>10</v>
-      </c>
-      <c r="F5">
-        <v>18</v>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s">
+        <v>11</v>
       </c>
       <c r="G5">
         <v>8</v>
@@ -505,20 +532,20 @@
       <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6">
-        <v>7</v>
-      </c>
-      <c r="C6">
-        <v>20</v>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
       </c>
       <c r="D6">
         <v>48</v>
       </c>
-      <c r="E6">
-        <v>12</v>
-      </c>
-      <c r="F6">
-        <v>18</v>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" t="s">
+        <v>11</v>
       </c>
       <c r="G6">
         <v>8</v>
@@ -528,11 +555,11 @@
       <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7">
-        <v>7</v>
-      </c>
-      <c r="C7">
-        <v>18</v>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
       </c>
       <c r="D7">
         <v>20</v>
@@ -545,11 +572,11 @@
       <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8">
-        <v>8</v>
-      </c>
-      <c r="C8">
-        <v>18</v>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
       </c>
       <c r="D8">
         <v>23</v>

</xml_diff>